<commit_message>
All lahx results in!
</commit_message>
<xml_diff>
--- a/BOTH.xlsx
+++ b/BOTH.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>problem</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t xml:space="preserve"> length</t>
+  </si>
+  <si>
+    <t>thx</t>
+  </si>
+  <si>
+    <t>tlahx</t>
+  </si>
+  <si>
+    <t>HX</t>
+  </si>
+  <si>
+    <t>LAHX</t>
   </si>
 </sst>
 </file>
@@ -150,6 +162,2276 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> graph of processing time against problem size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>HX</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$O$15:$O$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>127</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$15:$P$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>99.561078739166106</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>173.08408370017941</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>542.66534879207552</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>686.43687262535047</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>836.05227355956902</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-41D9-4372-9F6C-CADB5193F2AA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>LAHX</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$O$15:$O$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>127</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$15:$Q$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>195.1204630374904</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>325.6396948814388</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1356.3921173334079</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1276.0041848659457</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1977.8635812044092</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-41D9-4372-9F6C-CADB5193F2AA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="450975760"/>
+        <c:axId val="450975104"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="450975760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Problem</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> size</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="450975104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="450975104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time(s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="450975760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> graph of tour error against problem size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HX</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$O$15:$O$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>127</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$15:$R$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.5084681972149037</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.837037037037033</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.460916867932188</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.97628324580721</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.251111749885901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2CB3-42F4-AE7C-EA6E1558D16B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LAHX</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$O$15:$O$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>127</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$15:$S$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9.0459164471208098</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.12592592592593</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.395774552513373</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.694731492461472</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.604031044453084</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2CB3-42F4-AE7C-EA6E1558D16B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="450962312"/>
+        <c:axId val="450961328"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="450962312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Problem</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> size</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="450961328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="450961328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tour</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> error (%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="450962312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>176212</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>147637</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,10 +2755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:S75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15:S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +2766,7 @@
     <col min="7" max="7" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -513,7 +2795,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -523,8 +2805,230 @@
       <c r="C2">
         <v>10628</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>105.14611840248099</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>11631</v>
+      </c>
+      <c r="G2">
+        <v>192.05922627448999</v>
+      </c>
+      <c r="H2">
+        <v>17</v>
+      </c>
+      <c r="I2">
+        <v>11343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>84.183634281158405</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>11835</v>
+      </c>
+      <c r="G3">
+        <v>191.556301355361</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <v>11568</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>91.417138814926105</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>11395</v>
+      </c>
+      <c r="G4">
+        <v>200.698784589767</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <v>11410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>103.904840946197</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>11295</v>
+      </c>
+      <c r="G5">
+        <v>196.43670797348</v>
+      </c>
+      <c r="H5">
+        <v>17</v>
+      </c>
+      <c r="I5">
+        <v>12668</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>98.307477474212604</v>
+      </c>
+      <c r="E6">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>11087</v>
+      </c>
+      <c r="G6">
+        <v>200.816727638244</v>
+      </c>
+      <c r="H6">
+        <v>19</v>
+      </c>
+      <c r="I6">
+        <v>11238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>96.427776813506995</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>11471</v>
+      </c>
+      <c r="G7">
+        <v>185.73164010047901</v>
+      </c>
+      <c r="H7">
+        <v>13</v>
+      </c>
+      <c r="I7">
+        <v>11596</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>83.612838029861393</v>
+      </c>
+      <c r="E8">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>11011</v>
+      </c>
+      <c r="G8">
+        <v>164.64483165740899</v>
+      </c>
+      <c r="H8">
+        <v>13</v>
+      </c>
+      <c r="I8">
+        <v>12034</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>99.642042398452702</v>
+      </c>
+      <c r="E9">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>11552</v>
+      </c>
+      <c r="G9">
+        <v>151.27351927757201</v>
+      </c>
+      <c r="H9">
+        <v>13</v>
+      </c>
+      <c r="I9">
+        <v>11685</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>135.72395443916301</v>
+      </c>
+      <c r="E10">
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>11597</v>
+      </c>
+      <c r="G10">
+        <v>246.34779095649699</v>
+      </c>
+      <c r="H10">
+        <v>18</v>
+      </c>
+      <c r="I10">
+        <v>11288</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>(C11-C2)*100/C2</f>
+        <v>7.5084681972149037</v>
+      </c>
+      <c r="B11">
+        <f>AVERAGE(D2:D11)</f>
+        <v>99.561078739166135</v>
+      </c>
+      <c r="C11">
+        <f>AVERAGE(F2:F11)</f>
+        <v>11426</v>
+      </c>
+      <c r="D11">
+        <v>97.244965791702199</v>
+      </c>
+      <c r="E11">
+        <v>13</v>
+      </c>
+      <c r="F11">
+        <v>11386</v>
+      </c>
+      <c r="G11">
+        <v>221.639100551605</v>
+      </c>
+      <c r="H11">
+        <v>18</v>
+      </c>
+      <c r="I11">
+        <v>11064</v>
+      </c>
+      <c r="J11">
+        <f>AVERAGE(I2:I11)</f>
+        <v>11589.4</v>
+      </c>
+      <c r="K11">
+        <f>AVERAGE(G2:G11)</f>
+        <v>195.1204630374904</v>
+      </c>
+      <c r="L11">
+        <f>(J11-C2)*100/C2</f>
+        <v>9.0459164471208098</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -553,7 +3057,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>189.39427304267801</v>
       </c>
@@ -573,7 +3077,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>197.00321602821299</v>
       </c>
@@ -592,8 +3096,23 @@
       <c r="I14">
         <v>808</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>15</v>
+      </c>
+      <c r="P14" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>19</v>
+      </c>
+      <c r="R14" t="s">
+        <v>20</v>
+      </c>
+      <c r="S14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>194.73862409591601</v>
       </c>
@@ -612,8 +3131,23 @@
       <c r="I15">
         <v>822</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>48</v>
+      </c>
+      <c r="P15">
+        <v>99.561078739166106</v>
+      </c>
+      <c r="Q15">
+        <v>195.1204630374904</v>
+      </c>
+      <c r="R15">
+        <v>7.5084681972149037</v>
+      </c>
+      <c r="S15">
+        <v>9.0459164471208098</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>163.27473020553501</v>
       </c>
@@ -632,8 +3166,23 @@
       <c r="I16">
         <v>792</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <v>70</v>
+      </c>
+      <c r="P16">
+        <v>173.08408370017941</v>
+      </c>
+      <c r="Q16">
+        <v>325.6396948814388</v>
+      </c>
+      <c r="R16">
+        <v>15.837037037037033</v>
+      </c>
+      <c r="S16">
+        <v>17.12592592592593</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>142.79360222816399</v>
       </c>
@@ -652,8 +3201,23 @@
       <c r="I17">
         <v>748</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>107</v>
+      </c>
+      <c r="P17">
+        <v>542.66534879207552</v>
+      </c>
+      <c r="Q17">
+        <v>1356.3921173334079</v>
+      </c>
+      <c r="R17">
+        <v>30.460916867932188</v>
+      </c>
+      <c r="S17">
+        <v>22.395774552513373</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>150.98529362678499</v>
       </c>
@@ -672,8 +3236,23 @@
       <c r="I18">
         <v>759</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <v>124</v>
+      </c>
+      <c r="P18">
+        <v>686.43687262535047</v>
+      </c>
+      <c r="Q18">
+        <v>1276.0041848659457</v>
+      </c>
+      <c r="R18">
+        <v>47.97628324580721</v>
+      </c>
+      <c r="S18">
+        <v>44.694731492461472</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>175.247612476348</v>
       </c>
@@ -692,8 +3271,23 @@
       <c r="I19">
         <v>788</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>127</v>
+      </c>
+      <c r="P19">
+        <v>836.05227355956902</v>
+      </c>
+      <c r="Q19">
+        <v>1977.8635812044092</v>
+      </c>
+      <c r="R19">
+        <v>19.251111749885901</v>
+      </c>
+      <c r="S19">
+        <v>17.604031044453084</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>167.45141339302</v>
       </c>
@@ -713,7 +3307,15 @@
         <v>753</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f>(C21-C12)*100/C12</f>
+        <v>15.837037037037033</v>
+      </c>
+      <c r="B21">
+        <f>AVERAGE(D12:D21)</f>
+        <v>173.08408370017941</v>
+      </c>
       <c r="C21">
         <f>AVERAGE(F12:F21)</f>
         <v>781.9</v>
@@ -740,8 +3342,16 @@
         <f>AVERAGE(I12:I21)</f>
         <v>790.6</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <f>AVERAGE(G12:G21)</f>
+        <v>325.6396948814388</v>
+      </c>
+      <c r="L21">
+        <f>(J21-C12)*100/C12</f>
+        <v>17.12592592592593</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -770,7 +3380,7 @@
         <v>51813</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D23">
         <v>694.78396511077801</v>
       </c>
@@ -780,8 +3390,17 @@
       <c r="F23">
         <v>53531</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>1377.8828959465</v>
+      </c>
+      <c r="H23">
+        <v>49</v>
+      </c>
+      <c r="I23">
+        <v>50889</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D24">
         <v>377.011407852172</v>
       </c>
@@ -791,8 +3410,17 @@
       <c r="F24">
         <v>62848</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>1549.9904136657699</v>
+      </c>
+      <c r="H24">
+        <v>49</v>
+      </c>
+      <c r="I24">
+        <v>53257</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D25">
         <v>557.99196457862797</v>
       </c>
@@ -802,8 +3430,17 @@
       <c r="F25">
         <v>58955</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>1710.53624439239</v>
+      </c>
+      <c r="H25">
+        <v>52</v>
+      </c>
+      <c r="I25">
+        <v>54054</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>442.59872889518698</v>
       </c>
@@ -813,8 +3450,17 @@
       <c r="F26">
         <v>55015</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>900.74677705764702</v>
+      </c>
+      <c r="H26">
+        <v>33</v>
+      </c>
+      <c r="I26">
+        <v>58928</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>521.12663102149895</v>
       </c>
@@ -824,8 +3470,17 @@
       <c r="F27">
         <v>59680</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>1441.3375227451299</v>
+      </c>
+      <c r="H27">
+        <v>52</v>
+      </c>
+      <c r="I27">
+        <v>51568</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D28">
         <v>490.870854854583</v>
       </c>
@@ -835,8 +3490,17 @@
       <c r="F28">
         <v>62558</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>1347.84319472312</v>
+      </c>
+      <c r="H28">
+        <v>47</v>
+      </c>
+      <c r="I28">
+        <v>53815</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>476.41234421730002</v>
       </c>
@@ -846,8 +3510,17 @@
       <c r="F29">
         <v>61697</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>1309.2113456725999</v>
+      </c>
+      <c r="H29">
+        <v>47</v>
+      </c>
+      <c r="I29">
+        <v>53762</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D30">
         <v>657.63698196411099</v>
       </c>
@@ -857,8 +3530,25 @@
       <c r="F30">
         <v>51088</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>738.97807407379105</v>
+      </c>
+      <c r="H30">
+        <v>32</v>
+      </c>
+      <c r="I30">
+        <v>61447</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f>(C31-C22)*100/C22</f>
+        <v>30.460916867932188</v>
+      </c>
+      <c r="B31">
+        <f>AVERAGE(D22:D31)</f>
+        <v>542.66534879207552</v>
+      </c>
       <c r="C31">
         <f>AVERAGE(F22:F31)</f>
         <v>57798.1</v>
@@ -872,12 +3562,29 @@
       <c r="F31">
         <v>57450</v>
       </c>
+      <c r="G31">
+        <v>1813.3507370948701</v>
+      </c>
+      <c r="H31">
+        <v>54</v>
+      </c>
+      <c r="I31">
+        <v>52717</v>
+      </c>
       <c r="J31">
         <f>AVERAGE(I22:I31)</f>
-        <v>51813</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>54225</v>
+      </c>
+      <c r="K31">
+        <f>AVERAGE(G22:G31)</f>
+        <v>1356.3921173334079</v>
+      </c>
+      <c r="L31">
+        <f>(J31-C22)*100/C22</f>
+        <v>22.395774552513373</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -887,8 +3594,230 @@
       <c r="C32">
         <v>59030</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>639.33828449249199</v>
+      </c>
+      <c r="E32">
+        <v>29</v>
+      </c>
+      <c r="F32">
+        <v>80959</v>
+      </c>
+      <c r="G32">
+        <v>957.70228433608997</v>
+      </c>
+      <c r="H32">
+        <v>31</v>
+      </c>
+      <c r="I32">
+        <v>88200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>571.80756497383095</v>
+      </c>
+      <c r="E33">
+        <v>25</v>
+      </c>
+      <c r="F33">
+        <v>86746</v>
+      </c>
+      <c r="G33">
+        <v>1532.54710102081</v>
+      </c>
+      <c r="H33">
+        <v>35</v>
+      </c>
+      <c r="I33">
+        <v>82438</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>739.48689007759003</v>
+      </c>
+      <c r="E34">
+        <v>26</v>
+      </c>
+      <c r="F34">
+        <v>87951</v>
+      </c>
+      <c r="G34">
+        <v>1260.5728800296699</v>
+      </c>
+      <c r="H34">
+        <v>31</v>
+      </c>
+      <c r="I34">
+        <v>84763</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>588.92199993133499</v>
+      </c>
+      <c r="E35">
+        <v>27</v>
+      </c>
+      <c r="F35">
+        <v>81900</v>
+      </c>
+      <c r="G35">
+        <v>1657.56559157371</v>
+      </c>
+      <c r="H35">
+        <v>34</v>
+      </c>
+      <c r="I35">
+        <v>79381</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>699.01202416419903</v>
+      </c>
+      <c r="E36">
+        <v>25</v>
+      </c>
+      <c r="F36">
+        <v>83060</v>
+      </c>
+      <c r="G36">
+        <v>1525.4374179839999</v>
+      </c>
+      <c r="H36">
+        <v>37</v>
+      </c>
+      <c r="I36">
+        <v>80031</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>829.93195605278004</v>
+      </c>
+      <c r="E37">
+        <v>28</v>
+      </c>
+      <c r="F37">
+        <v>88265</v>
+      </c>
+      <c r="G37">
+        <v>991.97948575019802</v>
+      </c>
+      <c r="H37">
+        <v>26</v>
+      </c>
+      <c r="I37">
+        <v>98527</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>831.66584134101799</v>
+      </c>
+      <c r="E38">
+        <v>35</v>
+      </c>
+      <c r="F38">
+        <v>85749</v>
+      </c>
+      <c r="G38">
+        <v>1031.25484490394</v>
+      </c>
+      <c r="H38">
+        <v>25</v>
+      </c>
+      <c r="I38">
+        <v>89116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>692.66762804985001</v>
+      </c>
+      <c r="E39">
+        <v>29</v>
+      </c>
+      <c r="F39">
+        <v>88289</v>
+      </c>
+      <c r="G39">
+        <v>1316.8494198322201</v>
+      </c>
+      <c r="H39">
+        <v>35</v>
+      </c>
+      <c r="I39">
+        <v>85231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>818.45061707496598</v>
+      </c>
+      <c r="E40">
+        <v>25</v>
+      </c>
+      <c r="F40">
+        <v>88177</v>
+      </c>
+      <c r="G40">
+        <v>1300.03394484519</v>
+      </c>
+      <c r="H40">
+        <v>35</v>
+      </c>
+      <c r="I40">
+        <v>82556</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f>(C41-C32)*100/C32</f>
+        <v>47.97628324580721</v>
+      </c>
+      <c r="B41">
+        <f>AVERAGE(D32:D41)</f>
+        <v>686.43687262535047</v>
+      </c>
+      <c r="C41">
+        <f>AVERAGE(F32:F41)</f>
+        <v>87350.399999999994</v>
+      </c>
+      <c r="D41">
+        <v>453.08592009544299</v>
+      </c>
+      <c r="E41">
+        <v>15</v>
+      </c>
+      <c r="F41">
+        <v>102408</v>
+      </c>
+      <c r="G41">
+        <v>1186.0988783836301</v>
+      </c>
+      <c r="H41">
+        <v>35</v>
+      </c>
+      <c r="I41">
+        <v>83890</v>
+      </c>
+      <c r="J41">
+        <f>AVERAGE(I32:I41)</f>
+        <v>85413.3</v>
+      </c>
+      <c r="K41">
+        <f>AVERAGE(G32:G41)</f>
+        <v>1276.0041848659457</v>
+      </c>
+      <c r="L41">
+        <f>(J41-C32)*100/C32</f>
+        <v>44.694731492461472</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -898,8 +3827,230 @@
       <c r="C42">
         <v>118282</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>118282</v>
+      </c>
+      <c r="E42">
+        <v>891.08351445198002</v>
+      </c>
+      <c r="F42">
+        <v>24</v>
+      </c>
+      <c r="G42">
+        <v>1612.21561956405</v>
+      </c>
+      <c r="H42">
+        <v>39</v>
+      </c>
+      <c r="I42">
+        <v>141480</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>142693</v>
+      </c>
+      <c r="E43">
+        <v>780.47436475753705</v>
+      </c>
+      <c r="F43">
+        <v>25</v>
+      </c>
+      <c r="G43">
+        <v>5021.9402489662098</v>
+      </c>
+      <c r="H43">
+        <v>36</v>
+      </c>
+      <c r="I43">
+        <v>136655</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>146085</v>
+      </c>
+      <c r="E44">
+        <v>763.24476528167702</v>
+      </c>
+      <c r="F44">
+        <v>26</v>
+      </c>
+      <c r="G44">
+        <v>1647.1579895019499</v>
+      </c>
+      <c r="H44">
+        <v>45</v>
+      </c>
+      <c r="I44">
+        <v>145380</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>151028</v>
+      </c>
+      <c r="E45">
+        <v>852.80324149131695</v>
+      </c>
+      <c r="F45">
+        <v>27</v>
+      </c>
+      <c r="G45">
+        <v>1557.22236967086</v>
+      </c>
+      <c r="H45">
+        <v>42</v>
+      </c>
+      <c r="I45">
+        <v>142710</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>140956</v>
+      </c>
+      <c r="E46">
+        <v>811.24933195114102</v>
+      </c>
+      <c r="F46">
+        <v>27</v>
+      </c>
+      <c r="G46">
+        <v>1786.6236956119501</v>
+      </c>
+      <c r="H46">
+        <v>51</v>
+      </c>
+      <c r="I46">
+        <v>136332</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>142112</v>
+      </c>
+      <c r="E47">
+        <v>742.33379650115899</v>
+      </c>
+      <c r="F47">
+        <v>28</v>
+      </c>
+      <c r="G47">
+        <v>1758.1492319107001</v>
+      </c>
+      <c r="H47">
+        <v>53</v>
+      </c>
+      <c r="I47">
+        <v>138126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>143221</v>
+      </c>
+      <c r="E48">
+        <v>882.31979990005402</v>
+      </c>
+      <c r="F48">
+        <v>30</v>
+      </c>
+      <c r="G48">
+        <v>1704.670119524</v>
+      </c>
+      <c r="H48">
+        <v>47</v>
+      </c>
+      <c r="I48">
+        <v>141375</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>150057</v>
+      </c>
+      <c r="E49">
+        <v>886.35209178924504</v>
+      </c>
+      <c r="F49">
+        <v>30</v>
+      </c>
+      <c r="G49">
+        <v>1767.4909396171499</v>
+      </c>
+      <c r="H49">
+        <v>50</v>
+      </c>
+      <c r="I49">
+        <v>133095</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>138760</v>
+      </c>
+      <c r="E50">
+        <v>740.41022992134003</v>
+      </c>
+      <c r="F50">
+        <v>28</v>
+      </c>
+      <c r="G50">
+        <v>1351.9115569591499</v>
+      </c>
+      <c r="H50">
+        <v>33</v>
+      </c>
+      <c r="I50">
+        <v>133035</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f>(C51-C42)*100/C42</f>
+        <v>19.251111749885869</v>
+      </c>
+      <c r="B51">
+        <f>AVERAGE(E42:E51)</f>
+        <v>836.05227355956902</v>
+      </c>
+      <c r="C51">
+        <f>AVERAGE(D42:D51)</f>
+        <v>141052.6</v>
+      </c>
+      <c r="D51">
+        <v>137332</v>
+      </c>
+      <c r="E51">
+        <v>1010.25159955024</v>
+      </c>
+      <c r="F51">
+        <v>32</v>
+      </c>
+      <c r="G51">
+        <v>1571.25404071807</v>
+      </c>
+      <c r="H51">
+        <v>38</v>
+      </c>
+      <c r="I51">
+        <v>142856</v>
+      </c>
+      <c r="J51">
+        <f>AVERAGE(I42:I51)</f>
+        <v>139104.4</v>
+      </c>
+      <c r="K51">
+        <f>AVERAGE(G42:G51)</f>
+        <v>1977.8635812044092</v>
+      </c>
+      <c r="L51">
+        <f>(J51-C42)*100/C42</f>
+        <v>17.604031044453084</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -910,7 +4061,7 @@
         <v>96772</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -970,6 +4121,8 @@
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>